<commit_message>
GreenCard update and Diagrama de micro-arqui
</commit_message>
<xml_diff>
--- a/Green card.xlsx
+++ b/Green card.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="9KTmz/aAjRN1h2cx8kYBOEKrAvXeyKaT5ZmHGKgsqMo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="21eoDxfKgXTDK9KMKbZwwrsFnNIf5ySuWx8+HP7tx/c="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>Arquitectura de Computadores II - II Semestre 2023</t>
   </si>
@@ -52,22 +52,38 @@
     <t>Arithmetic</t>
   </si>
   <si>
+    <t>ADD Scalar</t>
+  </si>
+  <si>
+    <t>G6_ADDSCAL</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>G6_ADD r0 r1, r2</t>
+  </si>
+  <si>
+    <t>r0 = r1+ r2</t>
+  </si>
+  <si>
+    <t>3 operands instruction</t>
+  </si>
+  <si>
+    <t>Arithmetic
+Vectorial</t>
+  </si>
+  <si>
     <t>ADD</t>
   </si>
   <si>
     <t>G6_ADD</t>
   </si>
   <si>
-    <t>0000</t>
-  </si>
-  <si>
-    <t>G6_ADD r0 r1, r2</t>
-  </si>
-  <si>
-    <t>r0 = r1+ r2</t>
-  </si>
-  <si>
-    <t>3 operands instruction</t>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>r0 = r1+ r2; with r1 and r2 vectors</t>
   </si>
   <si>
     <t>SUB</t>
@@ -76,7 +92,7 @@
     <t>G6_SUB</t>
   </si>
   <si>
-    <t>0001</t>
+    <t>0010</t>
   </si>
   <si>
     <t>G6_SUB r0, r1, r2</t>
@@ -91,7 +107,7 @@
     <t>G6_EXP</t>
   </si>
   <si>
-    <t>0010</t>
+    <t>0011</t>
   </si>
   <si>
     <t>G6_EXP r0, r1, r2</t>
@@ -106,7 +122,7 @@
     <t>G6_MULT</t>
   </si>
   <si>
-    <t>0011</t>
+    <t>0100</t>
   </si>
   <si>
     <t>G6_MULT r0, r1, r2</t>
@@ -121,7 +137,7 @@
     <t>G6_CMP</t>
   </si>
   <si>
-    <t>0100</t>
+    <t>0101</t>
   </si>
   <si>
     <t>G6_CMP r1,r2</t>
@@ -142,7 +158,7 @@
     <t>G6_MOVI</t>
   </si>
   <si>
-    <t>0101</t>
+    <t>0110</t>
   </si>
   <si>
     <t>G6_MOVI r0, #0x150</t>
@@ -157,7 +173,7 @@
     <t>G6_MOVR</t>
   </si>
   <si>
-    <t>0110</t>
+    <t>0111</t>
   </si>
   <si>
     <t>G6_MOVR r0, r1</t>
@@ -175,7 +191,7 @@
     <t>G6_IDX</t>
   </si>
   <si>
-    <t>0111</t>
+    <t>1000</t>
   </si>
   <si>
     <t>G6_IDX x_values, r0, r1</t>
@@ -190,7 +206,7 @@
     <t>G6_APPEND</t>
   </si>
   <si>
-    <t>1000</t>
+    <t>1001</t>
   </si>
   <si>
     <t>G6_APPEND x_values, r0</t>
@@ -199,6 +215,36 @@
     <t>Add the value of r0 to x_values</t>
   </si>
   <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>G6_BEQ</t>
+  </si>
+  <si>
+    <t>G6_BEQ tag</t>
+  </si>
+  <si>
+    <t>Jumps to the tag if the branch flag is up</t>
+  </si>
+  <si>
+    <t>1 operand instruction</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>G6_B</t>
+  </si>
+  <si>
+    <t>G6_B tag</t>
+  </si>
+  <si>
+    <t>Jumps to the tag</t>
+  </si>
+  <si>
     <t>Control</t>
   </si>
   <si>
@@ -208,24 +254,24 @@
     <t>G6_LDR</t>
   </si>
   <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>G6_LDR r0, r1</t>
+  </si>
+  <si>
+    <t>Load the value from memory at r1 into r0</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>G6_STR</t>
+  </si>
+  <si>
     <t>1101</t>
   </si>
   <si>
-    <t>G6_LDR r0, r1</t>
-  </si>
-  <si>
-    <t>Load the value from memory at r1 into r0</t>
-  </si>
-  <si>
-    <t>STR</t>
-  </si>
-  <si>
-    <t>G6_STR</t>
-  </si>
-  <si>
-    <t>1011</t>
-  </si>
-  <si>
     <t>G6_STR r0, [r1]</t>
   </si>
   <si>
@@ -241,14 +287,14 @@
     <t>16 bits</t>
   </si>
   <si>
-    <t>12 registros uso general</t>
+    <t>8 registros uso general</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -284,6 +330,11 @@
     </font>
     <font/>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -362,6 +413,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -373,10 +427,18 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -390,28 +452,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -421,6 +461,14 @@
         <color rgb="FF000000"/>
       </right>
       <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
@@ -428,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -462,94 +510,110 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -768,7 +832,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="6.71"/>
     <col customWidth="1" min="2" max="2" width="10.29"/>
-    <col customWidth="1" min="3" max="3" width="9.86"/>
+    <col customWidth="1" min="3" max="3" width="10.57"/>
     <col customWidth="1" min="4" max="4" width="13.71"/>
     <col customWidth="1" min="5" max="5" width="10.43"/>
     <col customWidth="1" min="6" max="6" width="23.0"/>
@@ -839,28 +903,30 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="13"/>
+      <c r="B9" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="F9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="13"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
@@ -870,18 +936,18 @@
       <c r="E10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="13"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="8" t="s">
         <v>27</v>
       </c>
@@ -891,199 +957,261 @@
       <c r="E11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="8" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="22" t="s">
-        <v>37</v>
+      <c r="H12" s="17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="F13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="G13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>42</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="28" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="18"/>
-      <c r="C14" s="29" t="s">
+      <c r="B14" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="32" t="s">
-        <v>37</v>
+      <c r="H14" s="29" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="E15" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="F15" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="G15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="37" t="s">
-        <v>54</v>
-      </c>
       <c r="H15" s="34" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="32" t="s">
-        <v>37</v>
+      <c r="H16" s="36" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="D17" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="E17" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="F17" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="G17" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="40" t="s">
-        <v>37</v>
+      <c r="H17" s="34" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="18"/>
+      <c r="B18" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="C18" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="42">
+        <v>1010.0</v>
+      </c>
+      <c r="F18" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="G18" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="43" t="s">
+    <row r="19">
+      <c r="B19" s="30"/>
+      <c r="C19" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D19" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>72</v>
+      <c r="E19" s="42">
+        <v>1011.0</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>74</v>
+    <row r="20">
+      <c r="B20" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="30"/>
+      <c r="C21" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="C23" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="50" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -2054,12 +2182,14 @@
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
     <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B17:B18"/>
+  <mergeCells count="5">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>